<commit_message>
added signup but broke again
</commit_message>
<xml_diff>
--- a/quiz-questions.xlsx
+++ b/quiz-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\enneagram-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E1B26A-473F-4F02-A7E6-5BD4F14A77A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F5502C-2785-49FC-BB00-38FF819D7150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -59,31 +59,7 @@
     <t>Reflects Type 1’s perfectionism and internal self-criticism. This explores their inner drive for improvement.</t>
   </si>
   <si>
-    <t>"I feel unsettled when things don’t meet my standards of order and correctness."</t>
-  </si>
-  <si>
-    <t>Highlights Type 1's focus on structure and aversion to chaos.</t>
-  </si>
-  <si>
-    <t>Addresses Type 1’s adherence to principles and their tendency to see the world in terms of right and wrong.</t>
-  </si>
-  <si>
-    <t>"I feel frustrated when things or people don’t live up to the standards I hold."</t>
-  </si>
-  <si>
-    <t>"I often neglect my own needs because I feel fulfilled when I’m making others feel loved and supported."</t>
-  </si>
-  <si>
-    <t>Explores Type 2’s core motivation to be loved and valued through helpfulness and connection. This emphasizes their tendency to derive self-worth from being indispensable.</t>
-  </si>
-  <si>
     <t>"I tend to feel a moral obligation to meet higher standards than I expect from others."</t>
-  </si>
-  <si>
-    <t>"I feel an inner pressure to improve things and hold myself to a higher standard than I expect from others, even when no one is watching."</t>
-  </si>
-  <si>
-    <t>"I constantly notice flaws, inefficiencies, and ways things could be improved, and I feel a responsibility to fix them. It frustrates me when others don't seem to care about doing things the right way."</t>
   </si>
 </sst>
 </file>
@@ -404,7 +380,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -454,7 +430,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -464,66 +440,34 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="4">
-        <v>6</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4">
-        <v>7</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5">
-        <v>8</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5">
-        <v>9</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>